<commit_message>
Added MyExcelUtilities project with a "grabber" class.
git-svn-id: file:///Users/ken/Repository/biomedken/trunk/csharp_sandbox@164 ab604922-b16d-4620-a341-c5f183439689
</commit_message>
<xml_diff>
--- a/ExcelWorkbookTestDataSource/ExcelWorkbookTestDataSource/testDataSource.xlsx
+++ b/ExcelWorkbookTestDataSource/ExcelWorkbookTestDataSource/testDataSource.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11340" windowHeight="6765"/>
+    <workbookView xWindow="423" yWindow="4129" windowWidth="14400" windowHeight="5136"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="LookupTable">Sheet1!$A$1:$C$4</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>KEY</t>
-  </si>
-  <si>
-    <t>VALUE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>basePath</t>
   </si>
@@ -36,13 +32,22 @@
     <t>C:\Program Files\mricron\MRIcroN.exe</t>
   </si>
   <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>again</t>
-  </si>
-  <si>
-    <t>something</t>
+    <t>pADATremap</t>
+  </si>
+  <si>
+    <t>.\masked_roi98_mniwholebrain_fromspm_wroi99_wholecube_both_p-overlay_adathreshold_remap_clustercorrected.hdr</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>nextAbbrevOverlay</t>
+  </si>
+  <si>
+    <t>.\next\goes\here</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -60,18 +65,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,17 +99,15 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,57 +404,61 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -456,21 +469,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
+  <cols>
+    <col min="1" max="1" width="86.453125" customWidth="1"/>
+  </cols>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>